<commit_message>
process 20200723 data. Too small of an effect for the selection
</commit_message>
<xml_diff>
--- a/code/processing/growth_curves_plate_reader/20200723_r1_O1_ST_tetracycline-sucrose/20200723_plate_layout.xlsx
+++ b/code/processing/growth_curves_plate_reader/20200723_r1_O1_ST_tetracycline-sucrose/20200723_plate_layout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrazomej/git/evo_mwc/code/processing/growth_curves_plate_reader/20200723_r1_O1_ST_tetracycline-sucrose/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C060AE54-594F-0D4F-9BED-539A2CB6FFB8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE6F5D4D-50F1-2F40-A3D5-0EAFB381FDE1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="23620" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38300" windowHeight="23620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="strain" sheetId="1" r:id="rId1"/>
@@ -223,9 +223,6 @@
     <t>0.5_%wv_surcorse</t>
   </si>
   <si>
-    <t>none_HG105_none_mCh</t>
-  </si>
-  <si>
     <t>O2_R0_ST_mCh</t>
   </si>
   <si>
@@ -236,6 +233,9 @@
   </si>
   <si>
     <t>O2_R1740_ST_mCh</t>
+  </si>
+  <si>
+    <t>none_R0_none_mCh</t>
   </si>
 </sst>
 </file>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,132 +615,132 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -976,7 +976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>

</xml_diff>